<commit_message>
locode example as .xlsx and unpacked structure - updated
</commit_message>
<xml_diff>
--- a/locode/locode example.xlsx
+++ b/locode/locode example.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malik\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malik\Documents\Repositories\TestRepo\locode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9BB0A553-74AF-463A-B1FB-F604EB5022F2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C22BC29F-1173-4334-B21D-2A43EE409009}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7440" xr2:uid="{41F897B0-C28E-4B75-8622-137A02EEBB35}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="105">
   <si>
     <t>Ch</t>
   </si>
@@ -144,9 +144,6 @@
     <t>WI </t>
   </si>
   <si>
-    <t>+ </t>
-  </si>
-  <si>
     <t>US  9AB </t>
   </si>
   <si>
@@ -334,6 +331,15 @@
   </si>
   <si>
     <t>3508N 07925W </t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>Abeerdeen </t>
   </si>
 </sst>
 </file>
@@ -729,7 +735,7 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -973,19 +979,19 @@
     </row>
     <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>42</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>14</v>
@@ -994,27 +1000,27 @@
         <v>15</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I9" s="3"/>
       <c r="J9" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K9" s="3"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="D10" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>47</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>14</v>
@@ -1023,56 +1029,58 @@
         <v>15</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I10" s="3"/>
       <c r="J10" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="K10" s="3"/>
+    </row>
+    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="K10" s="3"/>
-    </row>
-    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>51</v>
-      </c>
       <c r="D11" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>20</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>26</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I11" s="3"/>
       <c r="J11" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K11" s="3"/>
     </row>
     <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="D12" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>57</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>14</v>
@@ -1085,23 +1093,23 @@
       </c>
       <c r="I12" s="3"/>
       <c r="J12" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K12" s="3"/>
     </row>
     <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="D13" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>61</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>14</v>
@@ -1114,52 +1122,52 @@
       </c>
       <c r="I13" s="3"/>
       <c r="J13" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K13" s="3"/>
     </row>
     <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C14" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>65</v>
-      </c>
       <c r="F14" s="3" t="s">
-        <v>14</v>
+        <v>93</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I14" s="3"/>
       <c r="J14" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K14" s="3"/>
     </row>
     <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>69</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>14</v>
@@ -1177,16 +1185,16 @@
     <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>71</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>14</v>
@@ -1195,36 +1203,36 @@
         <v>15</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I16" s="3"/>
       <c r="J16" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K16" s="3"/>
     </row>
     <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E17" s="3" t="s">
+      <c r="F17" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="G17" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="H17" s="3" t="s">
         <v>77</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>78</v>
       </c>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
@@ -1233,45 +1241,45 @@
     <row r="18" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E18" s="3" t="s">
+      <c r="F18" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>81</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I18" s="3"/>
       <c r="J18" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K18" s="3"/>
     </row>
     <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>85</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>14</v>
@@ -1280,53 +1288,53 @@
         <v>15</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I19" s="3"/>
       <c r="J19" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K19" s="3"/>
     </row>
     <row r="20" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>88</v>
-      </c>
       <c r="F20" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I20" s="3"/>
       <c r="J20" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K20" s="3"/>
     </row>
     <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>31</v>
@@ -1347,77 +1355,77 @@
     <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E22" s="3" t="s">
+      <c r="F22" s="3" t="s">
         <v>93</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>94</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I22" s="3"/>
       <c r="J22" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K22" s="3"/>
     </row>
     <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>33</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I23" s="3"/>
       <c r="J23" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K23" s="3"/>
     </row>
     <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="D24" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F24" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>101</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>15</v>
@@ -1427,7 +1435,7 @@
       </c>
       <c r="I24" s="3"/>
       <c r="J24" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K24" s="3"/>
     </row>

</xml_diff>